<commit_message>
Esqueletos revisados contra manuscrito.
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado05/guion01/esqueletoGuion_LE_05_01_CO.xlsx
+++ b/fuentes/contenidos/grado05/guion01/esqueletoGuion_LE_05_01_CO.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="20225"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14180" tabRatio="729"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23256" windowHeight="13176" tabRatio="729"/>
   </bookViews>
   <sheets>
     <sheet name="GUION" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,11 @@
     <sheet name="CUADERNO DEL PROFESOR" sheetId="15" r:id="rId4"/>
     <sheet name="CUADERNO DE ESTUDIO" sheetId="16" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'CUADERNO DE ESTUDIO'!$A$1:$I$65</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'CUADERNO DEL PROFESOR'!$A$1:$C$26</definedName>
+  </definedNames>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -26,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="76">
   <si>
     <t>FICHA</t>
   </si>
@@ -91,9 +95,6 @@
     <t>LE_05_01_CO</t>
   </si>
   <si>
-    <t>Descubre qué es un relato literario y sus clases, qué es una novela y un cuento y cúales son sus características distinitivas.</t>
-  </si>
-  <si>
     <t>Lenguaje</t>
   </si>
   <si>
@@ -250,10 +251,13 @@
     <t>Antología de relatos literarios</t>
   </si>
   <si>
-    <t>Más información</t>
-  </si>
-  <si>
     <t>Educación Básica Primaria</t>
+  </si>
+  <si>
+    <t>Descubre qué es un relato literario y sus clases, qué es una novela y un cuento y cuáles son sus características distinitivas.</t>
+  </si>
+  <si>
+    <t>Fin de la unidad</t>
   </si>
 </sst>
 </file>
@@ -314,7 +318,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -333,8 +337,50 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC99FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -355,6 +401,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="595">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -953,7 +1014,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -970,10 +1031,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -988,6 +1045,68 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="595">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
@@ -1588,6 +1707,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFCC99FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1864,66 +1988,67 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.5" customWidth="1"/>
+    <col min="1" max="1" width="22.44140625" customWidth="1"/>
     <col min="2" max="2" width="104.33203125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
         <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="15" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="13" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="15" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="13" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="15" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="13" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="13" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="15" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="13" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1936,57 +2061,60 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="64.6640625" customWidth="1"/>
-    <col min="5" max="5" width="20.5" customWidth="1"/>
+    <col min="1" max="1" width="4.109375" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.77734375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.88671875" customWidth="1"/>
+    <col min="9" max="10" width="15.109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="18.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="16.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="12" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="4" customFormat="1">
+    <row r="2" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>5</v>
       </c>
       <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" t="s">
         <v>23</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>24</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>25</v>
-      </c>
-      <c r="E2" t="s">
-        <v>26</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -1998,117 +2126,117 @@
       <c r="K2"/>
       <c r="L2"/>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>5</v>
       </c>
       <c r="B3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" t="s">
         <v>23</v>
       </c>
-      <c r="C3" t="s">
-        <v>24</v>
-      </c>
       <c r="D3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>5</v>
       </c>
       <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" t="s">
         <v>23</v>
       </c>
-      <c r="C4" t="s">
-        <v>24</v>
-      </c>
       <c r="D4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>5</v>
       </c>
       <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
         <v>23</v>
       </c>
-      <c r="C5" t="s">
-        <v>24</v>
-      </c>
       <c r="D5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F5">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s">
         <v>23</v>
       </c>
-      <c r="C6" t="s">
-        <v>24</v>
-      </c>
       <c r="D6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F6">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" t="s">
         <v>23</v>
       </c>
-      <c r="C7" t="s">
-        <v>24</v>
-      </c>
       <c r="D7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F7">
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
-      <c r="G9" s="10"/>
-    </row>
-    <row r="10" spans="1:12">
-      <c r="G10" s="10"/>
-    </row>
-    <row r="11" spans="1:12">
-      <c r="G11" s="10"/>
-    </row>
-    <row r="12" spans="1:12">
-      <c r="G12" s="10"/>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="G9" s="8"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="G10" s="8"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="G11" s="8"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="G12" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2124,231 +2252,232 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:A20"/>
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="66.1640625" customWidth="1"/>
+    <col min="1" max="1" width="37.21875" customWidth="1"/>
     <col min="2" max="2" width="14.6640625" customWidth="1"/>
+    <col min="3" max="4" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="12" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="4" customFormat="1">
+    <row r="2" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C2">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="4" customFormat="1">
+    <row r="3" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="4" customFormat="1">
+    <row r="4" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C4">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="4" customFormat="1">
+    <row r="5" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C5">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C6">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C7">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C8">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C9">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C10">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C11">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C12">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C13">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C14">
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>46</v>
       </c>
-      <c r="B15" t="s">
-        <v>33</v>
-      </c>
-      <c r="C15">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" t="s">
-        <v>47</v>
-      </c>
       <c r="B16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C16">
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C17">
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" t="s">
         <v>49</v>
-      </c>
-      <c r="B18" t="s">
-        <v>50</v>
       </c>
       <c r="C18">
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C19">
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C20">
         <v>25</v>
@@ -2374,304 +2503,304 @@
   </sheetPr>
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="92.33203125" customWidth="1"/>
     <col min="3" max="3" width="19.33203125" style="7" customWidth="1"/>
-    <col min="4" max="4" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
         <v>45</v>
       </c>
-      <c r="C19" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20">
-        <v>19</v>
-      </c>
-      <c r="B20" t="s">
-        <v>46</v>
-      </c>
       <c r="C20" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C27" s="6"/>
     </row>
   </sheetData>
@@ -2692,1113 +2821,1314 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I65"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="70.1640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="28.33203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="61.33203125" style="3" customWidth="1"/>
-    <col min="5" max="7" width="17.83203125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="64.1640625" customWidth="1"/>
-    <col min="9" max="9" width="17.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35" style="2" customWidth="1"/>
+    <col min="3" max="3" width="15.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="42.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="38.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.77734375" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="15" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
-      <c r="A2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" s="8" t="s">
+    <row r="2" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+    </row>
+    <row r="3" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="5"/>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="8" t="s">
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="27"/>
+    </row>
+    <row r="4" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+    </row>
+    <row r="5" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="5"/>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" s="8" t="s">
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" s="27" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="27"/>
+    </row>
+    <row r="7" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="I7" s="27" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="25"/>
+      <c r="D8" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="27"/>
+    </row>
+    <row r="9" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="25"/>
+      <c r="D9" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="5"/>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" s="8" t="s">
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="27"/>
+      <c r="I9" s="27"/>
+    </row>
+    <row r="10" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="25"/>
+      <c r="D10" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="F10" s="26"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="27"/>
+      <c r="I10" s="27"/>
+    </row>
+    <row r="11" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="25"/>
+      <c r="D11" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="27"/>
+      <c r="I11" s="27"/>
+    </row>
+    <row r="12" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="25"/>
+      <c r="D12" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="F12" s="26"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="27"/>
+      <c r="I12" s="27"/>
+    </row>
+    <row r="13" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="25"/>
+      <c r="D13" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="F13" s="26"/>
+      <c r="G13" s="26"/>
+      <c r="H13" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="I13" s="27" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="25"/>
+      <c r="D14" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="I5" s="5" t="s">
+      <c r="F14" s="26"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="27"/>
+      <c r="I14" s="27"/>
+    </row>
+    <row r="15" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="25"/>
+      <c r="D15" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="E15" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="F15" s="26"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="27"/>
+      <c r="I15" s="27"/>
+    </row>
+    <row r="16" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="25"/>
+      <c r="D16" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="E16" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="F16" s="26"/>
+      <c r="G16" s="26"/>
+      <c r="H16" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="I16" s="26" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="25"/>
+      <c r="D17" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="E17" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="F17" s="26"/>
+      <c r="G17" s="26"/>
+      <c r="H17" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="I17" s="26" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="19"/>
+      <c r="I18" s="19"/>
+    </row>
+    <row r="19" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="19"/>
+      <c r="I19" s="19"/>
+    </row>
+    <row r="20" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="19"/>
+      <c r="I20" s="19"/>
+    </row>
+    <row r="21" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="I21" s="19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="19"/>
+      <c r="I22" s="19"/>
+    </row>
+    <row r="23" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" s="17"/>
+      <c r="D23" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="E23" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="19"/>
+      <c r="I23" s="19"/>
+    </row>
+    <row r="24" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" s="17"/>
+      <c r="D24" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="E24" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="I24" s="18" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B25" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" s="17"/>
+      <c r="D25" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="E25" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="19"/>
+      <c r="I25" s="19"/>
+    </row>
+    <row r="26" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B26" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26" s="17"/>
+      <c r="D26" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="E26" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="19"/>
+      <c r="I26" s="19"/>
+    </row>
+    <row r="27" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B27" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C27" s="17"/>
+      <c r="D27" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="E27" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="I27" s="18" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B28" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28" s="17"/>
+      <c r="D28" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E28" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
+    </row>
+    <row r="29" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B29" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C29" s="17"/>
+      <c r="D29" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E29" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
+      <c r="H29" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="I29" s="18" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="B30" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="C30" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="D30" s="30"/>
+      <c r="E30" s="30"/>
+      <c r="F30" s="30"/>
+      <c r="G30" s="30"/>
+      <c r="H30" s="31"/>
+      <c r="I30" s="31"/>
+    </row>
+    <row r="31" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="B31" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="C31" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="D31" s="30"/>
+      <c r="E31" s="30"/>
+      <c r="F31" s="30"/>
+      <c r="G31" s="30"/>
+      <c r="H31" s="31"/>
+      <c r="I31" s="31"/>
+    </row>
+    <row r="32" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="B32" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="C32" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="D32" s="30"/>
+      <c r="E32" s="30"/>
+      <c r="F32" s="30"/>
+      <c r="G32" s="30"/>
+      <c r="H32" s="31"/>
+      <c r="I32" s="31"/>
+    </row>
+    <row r="33" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="B33" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="C33" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="D33" s="30"/>
+      <c r="E33" s="30"/>
+      <c r="F33" s="30"/>
+      <c r="G33" s="30"/>
+      <c r="H33" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="I33" s="31" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="B34" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="C34" s="29"/>
+      <c r="D34" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="E34" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="F34" s="30"/>
+      <c r="G34" s="30"/>
+      <c r="H34" s="31"/>
+      <c r="I34" s="31"/>
+    </row>
+    <row r="35" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="B35" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="C35" s="29"/>
+      <c r="D35" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="E35" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="F35" s="30"/>
+      <c r="G35" s="30"/>
+      <c r="H35" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="I35" s="30" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="B36" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="C36" s="29"/>
+      <c r="D36" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="E36" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="F36" s="30"/>
+      <c r="G36" s="30"/>
+      <c r="H36" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="I36" s="31" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="B37" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="C37" s="29"/>
+      <c r="D37" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="E37" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="F37" s="30"/>
+      <c r="G37" s="30"/>
+      <c r="H37" s="31"/>
+      <c r="I37" s="31"/>
+    </row>
+    <row r="38" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="B38" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="C38" s="29"/>
+      <c r="D38" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="E38" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="F38" s="30"/>
+      <c r="G38" s="30"/>
+      <c r="H38" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="I38" s="30" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="B39" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="C39" s="29"/>
+      <c r="D39" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="E39" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="F39" s="30"/>
+      <c r="G39" s="30"/>
+      <c r="H39" s="31"/>
+      <c r="I39" s="31"/>
+    </row>
+    <row r="40" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="B40" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="C40" s="29"/>
+      <c r="D40" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="E40" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="F40" s="30"/>
+      <c r="G40" s="30"/>
+      <c r="H40" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="I40" s="31" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="B41" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="C41" s="29"/>
+      <c r="D41" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="E41" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="F41" s="30"/>
+      <c r="G41" s="30"/>
+      <c r="H41" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="I41" s="31" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B42" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="C42" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="D42" s="22"/>
+      <c r="E42" s="22"/>
+      <c r="F42" s="22"/>
+      <c r="G42" s="22"/>
+      <c r="H42" s="23"/>
+      <c r="I42" s="23"/>
+    </row>
+    <row r="43" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B43" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="C43" s="21"/>
+      <c r="D43" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="E43" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="F43" s="22"/>
+      <c r="G43" s="22"/>
+      <c r="H43" s="23"/>
+      <c r="I43" s="23"/>
+    </row>
+    <row r="44" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B44" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="C44" s="21"/>
+      <c r="D44" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="E44" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="F44" s="22"/>
+      <c r="G44" s="22"/>
+      <c r="H44" s="23"/>
+      <c r="I44" s="23"/>
+    </row>
+    <row r="45" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B45" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="C45" s="21"/>
+      <c r="D45" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="E45" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="F45" s="22"/>
+      <c r="G45" s="22"/>
+      <c r="H45" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="I45" s="22" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B46" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="C46" s="21"/>
+      <c r="D46" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="E46" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="F46" s="22"/>
+      <c r="G46" s="22"/>
+      <c r="H46" s="23"/>
+      <c r="I46" s="23"/>
+    </row>
+    <row r="47" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B47" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="C47" s="21"/>
+      <c r="D47" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="E47" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="F47" s="22"/>
+      <c r="G47" s="22"/>
+      <c r="H47" s="23"/>
+      <c r="I47" s="23"/>
+    </row>
+    <row r="48" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B48" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="C48" s="21"/>
+      <c r="D48" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="E48" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="F48" s="22"/>
+      <c r="G48" s="22"/>
+      <c r="H48" s="23"/>
+      <c r="I48" s="23"/>
+    </row>
+    <row r="49" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B49" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="C49" s="21"/>
+      <c r="D49" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="E49" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="F49" s="22"/>
+      <c r="G49" s="22"/>
+      <c r="H49" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="I49" s="22" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B50" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="C50" s="21"/>
+      <c r="D50" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="E50" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="F50" s="22"/>
+      <c r="G50" s="22"/>
+      <c r="H50" s="23"/>
+      <c r="I50" s="23"/>
+    </row>
+    <row r="51" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B51" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="C51" s="21"/>
+      <c r="D51" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="E51" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="F51" s="22"/>
+      <c r="G51" s="22"/>
+      <c r="H51" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="I51" s="22" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="B52" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="C52" s="33" t="s">
+        <v>52</v>
+      </c>
+      <c r="D52" s="34"/>
+      <c r="E52" s="34"/>
+      <c r="F52" s="34"/>
+      <c r="G52" s="34"/>
+      <c r="H52" s="35"/>
+      <c r="I52" s="35"/>
+    </row>
+    <row r="53" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="B53" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="C53" s="33" t="s">
+        <v>56</v>
+      </c>
+      <c r="D53" s="34"/>
+      <c r="E53" s="34"/>
+      <c r="F53" s="34"/>
+      <c r="G53" s="34"/>
+      <c r="H53" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="I53" s="35" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="B54" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="C54" s="33" t="s">
+        <v>53</v>
+      </c>
+      <c r="D54" s="34"/>
+      <c r="E54" s="34"/>
+      <c r="F54" s="34"/>
+      <c r="G54" s="34"/>
+      <c r="H54" s="35"/>
+      <c r="I54" s="35"/>
+    </row>
+    <row r="55" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="B55" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="C55" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="D55" s="34"/>
+      <c r="E55" s="34"/>
+      <c r="F55" s="34"/>
+      <c r="G55" s="34"/>
+      <c r="H55" s="35"/>
+      <c r="I55" s="35"/>
+    </row>
+    <row r="56" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="B56" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="C56" s="33" t="s">
+        <v>52</v>
+      </c>
+      <c r="D56" s="34"/>
+      <c r="E56" s="34"/>
+      <c r="F56" s="34"/>
+      <c r="G56" s="34"/>
+      <c r="H56" s="35"/>
+      <c r="I56" s="35"/>
+    </row>
+    <row r="57" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="B57" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="C57" s="33"/>
+      <c r="D57" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="E57" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="F57" s="34"/>
+      <c r="G57" s="34"/>
+      <c r="H57" s="35"/>
+      <c r="I57" s="35"/>
+    </row>
+    <row r="58" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="B58" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="C58" s="33"/>
+      <c r="D58" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="E58" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="F58" s="34"/>
+      <c r="G58" s="34"/>
+      <c r="H58" s="35" t="s">
+        <v>46</v>
+      </c>
+      <c r="I58" s="35" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="B59" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="C59" s="33"/>
+      <c r="D59" s="34" t="s">
+        <v>59</v>
+      </c>
+      <c r="E59" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="F59" s="34"/>
+      <c r="G59" s="34"/>
+      <c r="H59" s="35"/>
+      <c r="I59" s="35"/>
+    </row>
+    <row r="60" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="B60" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="C60" s="33"/>
+      <c r="D60" s="34" t="s">
+        <v>59</v>
+      </c>
+      <c r="E60" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="F60" s="34"/>
+      <c r="G60" s="34"/>
+      <c r="H60" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="I60" s="35" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="B61" s="37" t="s">
+        <v>70</v>
+      </c>
+      <c r="C61" s="37" t="s">
+        <v>52</v>
+      </c>
+      <c r="D61" s="38"/>
+      <c r="E61" s="38"/>
+      <c r="F61" s="38"/>
+      <c r="G61" s="38"/>
+      <c r="H61" s="39"/>
+      <c r="I61" s="39"/>
+    </row>
+    <row r="62" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="B62" s="37" t="s">
+        <v>70</v>
+      </c>
+      <c r="C62" s="37" t="s">
+        <v>56</v>
+      </c>
+      <c r="D62" s="38"/>
+      <c r="E62" s="38"/>
+      <c r="F62" s="38"/>
+      <c r="G62" s="38"/>
+      <c r="H62" s="39" t="s">
+        <v>71</v>
+      </c>
+      <c r="I62" s="39" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="B63" s="37" t="s">
+        <v>70</v>
+      </c>
+      <c r="C63" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="D63" s="38"/>
+      <c r="E63" s="38"/>
+      <c r="F63" s="38"/>
+      <c r="G63" s="38"/>
+      <c r="H63" s="39" t="s">
+        <v>72</v>
+      </c>
+      <c r="I63" s="39" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="B64" s="41" t="s">
+        <v>75</v>
+      </c>
+      <c r="C64" s="41" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="5"/>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="I7" s="5" t="s">
+      <c r="D64" s="42"/>
+      <c r="E64" s="42"/>
+      <c r="F64" s="42"/>
+      <c r="G64" s="42"/>
+      <c r="H64" s="41" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="5"/>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="5"/>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="8"/>
-      <c r="D10" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="5"/>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="8"/>
-      <c r="D11" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="5"/>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="5"/>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="A13" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" s="8"/>
-      <c r="D13" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="I13" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="A14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="E14" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="5"/>
-    </row>
-    <row r="15" spans="1:9">
-      <c r="A15" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C15" s="8"/>
-      <c r="D15" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="E15" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="5"/>
-    </row>
-    <row r="16" spans="1:9">
-      <c r="A16" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C16" s="8"/>
-      <c r="D16" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="E16" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="I16" s="9" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9">
-      <c r="A17" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C17" s="8"/>
-      <c r="D17" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="E17" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="I17" s="9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9">
-      <c r="A18" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="5"/>
-    </row>
-    <row r="19" spans="1:9">
-      <c r="A19" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="5"/>
-    </row>
-    <row r="20" spans="1:9">
-      <c r="A20" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="5"/>
-    </row>
-    <row r="21" spans="1:9">
-      <c r="A21" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B21" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C21" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="I21" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9">
-      <c r="A22" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B22" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="5"/>
-    </row>
-    <row r="23" spans="1:9">
-      <c r="A23" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B23" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C23" s="8"/>
-      <c r="D23" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="E23" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="5"/>
-    </row>
-    <row r="24" spans="1:9">
-      <c r="A24" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C24" s="8"/>
-      <c r="D24" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="E24" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
-      <c r="H24" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="I24" s="9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9">
-      <c r="A25" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C25" s="8"/>
-      <c r="D25" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="E25" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="F25" s="9"/>
-      <c r="G25" s="9"/>
-      <c r="H25" s="5"/>
-    </row>
-    <row r="26" spans="1:9">
-      <c r="A26" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B26" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9">
-      <c r="A27" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="H27" t="s">
-        <v>35</v>
-      </c>
-      <c r="I27" s="9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9">
-      <c r="A28" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B28" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9">
-      <c r="A29" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B29" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="H29" t="s">
-        <v>36</v>
-      </c>
-      <c r="I29" s="9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9">
-      <c r="A30" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B30" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9">
-      <c r="A31" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B31" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9">
-      <c r="A32" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B32" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9">
-      <c r="A33" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B33" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="H33" t="s">
-        <v>37</v>
-      </c>
-      <c r="I33" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9">
-      <c r="A34" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B34" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9">
-      <c r="A35" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B35" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="H35" t="s">
-        <v>38</v>
-      </c>
-      <c r="I35" s="9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9">
-      <c r="A36" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B36" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E36" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="H36" t="s">
-        <v>39</v>
-      </c>
-      <c r="I36" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9">
-      <c r="A37" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B37" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9">
-      <c r="A38" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B38" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="H38" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="I38" s="9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9">
-      <c r="A39" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B39" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="E39" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9">
-      <c r="A40" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B40" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="E40" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="H40" t="s">
-        <v>41</v>
-      </c>
-      <c r="I40" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9">
-      <c r="A41" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B41" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="E41" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="H41" t="s">
-        <v>42</v>
-      </c>
-      <c r="I41" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9">
-      <c r="A42" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B42" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9">
-      <c r="A43" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B43" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9">
-      <c r="A44" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B44" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E44" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9">
-      <c r="A45" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B45" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E45" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="H45" t="s">
-        <v>43</v>
-      </c>
-      <c r="I45" s="9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9">
-      <c r="A46" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B46" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="D46" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E46" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9">
-      <c r="A47" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B47" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="D47" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E47" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9">
-      <c r="A48" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B48" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="D48" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E48" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9">
-      <c r="A49" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B49" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="D49" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E49" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="H49" t="s">
-        <v>44</v>
-      </c>
-      <c r="I49" s="9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9">
-      <c r="A50" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B50" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="E50" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9">
-      <c r="A51" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B51" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="D51" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="E51" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="H51" t="s">
-        <v>68</v>
-      </c>
-      <c r="I51" s="9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9">
-      <c r="A52" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B52" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9">
-      <c r="A53" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B53" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="H53" t="s">
-        <v>46</v>
-      </c>
-      <c r="I53" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9">
-      <c r="A54" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B54" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9">
-      <c r="A55" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B55" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9">
-      <c r="A56" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B56" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9">
-      <c r="A57" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B57" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="D57" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="E57" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9">
-      <c r="A58" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B58" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="D58" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="E58" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="H58" t="s">
-        <v>47</v>
-      </c>
-      <c r="I58" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9">
-      <c r="A59" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B59" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="D59" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="E59" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9">
-      <c r="A60" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B60" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="D60" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="E60" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="H60" t="s">
-        <v>48</v>
-      </c>
-      <c r="I60" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9">
-      <c r="A61" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B61" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9">
-      <c r="A62" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B62" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="H62" t="s">
-        <v>72</v>
-      </c>
-      <c r="I62" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9">
-      <c r="A63" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B63" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="H63" t="s">
-        <v>73</v>
-      </c>
-      <c r="I63" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9">
-      <c r="A64" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B64" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="C64" s="2" t="s">
+      <c r="I64" s="43" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="B65" s="41" t="s">
+        <v>75</v>
+      </c>
+      <c r="C65" s="41" t="s">
         <v>51</v>
       </c>
-      <c r="I64" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9">
-      <c r="A65" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B65" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="C65" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="H65" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="I65" s="5" t="s">
-        <v>33</v>
+      <c r="D65" s="42"/>
+      <c r="E65" s="42"/>
+      <c r="F65" s="42"/>
+      <c r="G65" s="42"/>
+      <c r="H65" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="I65" s="43" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>